<commit_message>
updating seed doc for prod
</commit_message>
<xml_diff>
--- a/main/data/MyCandidate Seed Doc.xlsx
+++ b/main/data/MyCandidate Seed Doc.xlsx
@@ -96,9 +96,6 @@
     <t>#F2AA71</t>
   </si>
   <si>
-    <t>G-tag script</t>
-  </si>
-  <si>
     <t>nav_bars_colour</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
 "national": {"file": "National.csv", "locator": ["list_type"]},
 "national_regional": {"file": "Regional.csv", "locator": ["list_type"]},
 }</t>
+  </si>
+  <si>
+    <t>gTag_script</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -490,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -517,16 +517,16 @@
         <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="U1" s="1"/>
     </row>
@@ -535,13 +535,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -555,7 +555,7 @@
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>19</v>
@@ -576,16 +576,16 @@
         <v>24</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="U2" s="1"/>
     </row>

</xml_diff>